<commit_message>
Added BDT and MET
</commit_message>
<xml_diff>
--- a/data/dots_test_def.xlsx
+++ b/data/dots_test_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\dots_home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF83CF9-3770-480B-9D29-AB048FA2D6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7635B3-F528-44A0-8B9E-8A5D933EF074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{490B3B89-1FDC-3A47-B429-BAF23A587403}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{490B3B89-1FDC-3A47-B429-BAF23A587403}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="476">
   <si>
     <t>name</t>
   </si>
@@ -1820,14 +1820,90 @@
   <si>
     <t>Der Beatwahrnehmungs-Test erfasst die Fähigkeit der Schüler, einen Beat innerhalb eines kurzen Musikausschnitts zu erkennen und zu bewerten. Jeder Musikausschnitt (Jazz, Rock oder orchestraler Pop) wird zweimal mit hinzugefügten Pieptönen abgespielt. Die Schüler müssen entscheiden, in welcher Version des Ausschnitts die Pieptöne außerhalb des Beats der Musik liegen.</t>
   </si>
+  <si>
+    <t>BDT</t>
+  </si>
+  <si>
+    <t>Beat Drop Test</t>
+  </si>
+  <si>
+    <t>Beat-Drop-Test</t>
+  </si>
+  <si>
+    <t>The BDT records the ability of the students to maintain an internal beat when it is missing in a musical stimulus.</t>
+  </si>
+  <si>
+    <t>http://testing.musikpsychologie.de/dots_demo_demo/?test=BDT</t>
+  </si>
+  <si>
+    <t>https://github.com/klausfrieler/BDT</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.3758/s13414-022-02592-2</t>
+  </si>
+  <si>
+    <t>Cinelyte, U., Cannon, J., Patel, A. D., &amp; Müllensiefen, D. (2022). Testing beat perception without sensory cues to the beat: The Beat-Drop Alignment Test (BDAT). Attention, Perception, &amp; Psychophysics. https://doi.org/10.3758/s13414-022-02592-2</t>
+  </si>
+  <si>
+    <t>Der Beat-Drop-Test erfasst die Fähigkeit der Schüler, innerlich einen Beat fortzuführen, wenn dieser im Stimulus fehlt.</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>Music Engagement Test</t>
+  </si>
+  <si>
+    <t>Fragebogen Musikalisches Engagement</t>
+  </si>
+  <si>
+    <t>The MET measures engagement with music.</t>
+  </si>
+  <si>
+    <t>7-point rating scale</t>
+  </si>
+  <si>
+    <t>http://testing.musikpsychologie.de/dots_demo_demo/?test=MET</t>
+  </si>
+  <si>
+    <t>http://www.davidmgreenberg.com/wp-content/uploads/2018/11/Greenberg-Rentfrow-escom-2015-Rules-of-engagement-The-structure-of-musical-engagement-and-its-personality-underpinnings-1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greenberg &amp; Rentfrow (2015). Rules of engagement: The structure of musical engagement and its personality underpinnings. IMCPC 10, Manchester
+</t>
+  </si>
+  <si>
+    <t>Der MET misst das Engagement mit Musik.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="29">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2025,27 +2101,36 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2054,52 +2139,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2108,17 +2175,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2436,108 +2513,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F4A50E-0F21-814A-93E2-91983839DCA8}">
-  <dimension ref="A1:R140"/>
+  <dimension ref="A1:R141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="5" customWidth="1"/>
-    <col min="2" max="3" width="31.5" style="5" customWidth="1"/>
-    <col min="4" max="5" width="13.875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="34.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="5" customWidth="1"/>
-    <col min="9" max="10" width="20.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="20.5" style="5" customWidth="1"/>
-    <col min="13" max="13" width="23.125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="22.5" style="5" customWidth="1"/>
-    <col min="15" max="15" width="31.375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="19.5" style="5" customWidth="1"/>
-    <col min="17" max="18" width="18.5" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="11" style="5"/>
+    <col min="1" max="1" width="13.625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="31.5" style="4" customWidth="1"/>
+    <col min="4" max="5" width="13.875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23" style="4" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="4" customWidth="1"/>
+    <col min="9" max="10" width="20.5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="20.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="23.125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.5" style="4" customWidth="1"/>
+    <col min="15" max="15" width="31.375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="19.5" style="4" customWidth="1"/>
+    <col min="17" max="18" width="18.5" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="21">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" s="6" customFormat="1" ht="21">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="21">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>387</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -2556,7 +2633,7 @@
       <c r="M2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="4" t="s">
         <v>271</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -2571,25 +2648,25 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="21">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>214</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -2621,25 +2698,25 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="21">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>181</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>403</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -2669,7 +2746,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="21">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2678,16 +2755,16 @@
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>215</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -2721,7 +2798,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="21">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2730,16 +2807,16 @@
       <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>272</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2757,11 +2834,11 @@
       <c r="M6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="7"/>
+      <c r="O6" s="6"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="21">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2770,16 +2847,16 @@
       <c r="C7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>273</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -2799,13 +2876,13 @@
         <v>19</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="7"/>
+      <c r="O7" s="6"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="21">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2814,16 +2891,16 @@
       <c r="C8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>216</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -2841,10 +2918,10 @@
       <c r="M8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="7"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:18" ht="21">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2853,16 +2930,16 @@
       <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>217</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -2880,10 +2957,10 @@
       <c r="M9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="7"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="21">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2892,16 +2969,16 @@
       <c r="C10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>218</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -2919,10 +2996,10 @@
       <c r="M10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="7"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="21">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2931,16 +3008,16 @@
       <c r="C11" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>219</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -2958,28 +3035,28 @@
       <c r="M11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="7"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="21">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>220</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -2999,7 +3076,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="7"/>
+      <c r="O12" s="6"/>
       <c r="P12" s="1" t="s">
         <v>24</v>
       </c>
@@ -3007,25 +3084,25 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="21">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>221</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -3054,30 +3131,30 @@
         <v>134</v>
       </c>
       <c r="Q13" s="2"/>
-      <c r="R13" s="18" t="s">
+      <c r="R13" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="21">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>185</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>389</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -3113,25 +3190,25 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="21">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>186</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>222</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -3165,25 +3242,25 @@
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="21">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>187</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>223</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -3215,25 +3292,25 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="21">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>412</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -3267,7 +3344,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="21">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3276,13 +3353,13 @@
       <c r="C18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="8" t="s">
         <v>237</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -3302,13 +3379,13 @@
         <v>97</v>
       </c>
       <c r="N18" s="1"/>
-      <c r="O18" s="7"/>
+      <c r="O18" s="6"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="3"/>
     </row>
     <row r="19" spans="1:18" ht="21">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3317,13 +3394,13 @@
       <c r="C19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="8" t="s">
         <v>237</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -3343,13 +3420,13 @@
         <v>97</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="7"/>
+      <c r="O19" s="6"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="3"/>
     </row>
     <row r="20" spans="1:18" ht="21">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3358,13 +3435,13 @@
       <c r="C20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>237</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -3384,13 +3461,13 @@
         <v>97</v>
       </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="7"/>
+      <c r="O20" s="6"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:18" ht="21">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -3399,13 +3476,13 @@
       <c r="C21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="8" t="s">
         <v>237</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -3425,13 +3502,13 @@
         <v>97</v>
       </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="7"/>
+      <c r="O21" s="6"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="3"/>
     </row>
     <row r="22" spans="1:18" ht="21">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -3440,13 +3517,13 @@
       <c r="C22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>237</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -3466,31 +3543,31 @@
         <v>97</v>
       </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="7"/>
+      <c r="O22" s="6"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="3"/>
     </row>
     <row r="23" spans="1:18" ht="21">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>413</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -3524,7 +3601,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="21">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3533,16 +3610,16 @@
       <c r="C24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="8" t="s">
         <v>224</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -3562,13 +3639,13 @@
         <v>13</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="7"/>
+      <c r="O24" s="6"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="3"/>
     </row>
     <row r="25" spans="1:18" ht="21">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -3577,16 +3654,16 @@
       <c r="C25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>274</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -3606,13 +3683,13 @@
         <v>13</v>
       </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="7"/>
+      <c r="O25" s="6"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="3"/>
     </row>
     <row r="26" spans="1:18" ht="21">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3621,16 +3698,16 @@
       <c r="C26" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>225</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -3650,13 +3727,13 @@
         <v>13</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="7"/>
+      <c r="O26" s="6"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="3"/>
     </row>
     <row r="27" spans="1:18" ht="21">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3665,16 +3742,16 @@
       <c r="C27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>275</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -3692,10 +3769,10 @@
       <c r="M27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O27" s="7"/>
+      <c r="O27" s="6"/>
     </row>
     <row r="28" spans="1:18" ht="21">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3704,16 +3781,16 @@
       <c r="C28" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>276</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -3731,10 +3808,10 @@
       <c r="M28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O28" s="7"/>
+      <c r="O28" s="6"/>
     </row>
     <row r="29" spans="1:18" ht="21">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -3743,16 +3820,16 @@
       <c r="C29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>277</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -3770,10 +3847,10 @@
       <c r="M29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O29" s="7"/>
+      <c r="O29" s="6"/>
     </row>
     <row r="30" spans="1:18" ht="21">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3782,16 +3859,16 @@
       <c r="C30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>226</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -3809,10 +3886,10 @@
       <c r="M30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O30" s="7"/>
+      <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:18" ht="21">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3821,16 +3898,16 @@
       <c r="C31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="7" t="s">
         <v>278</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -3848,10 +3925,10 @@
       <c r="M31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O31" s="7"/>
+      <c r="O31" s="6"/>
     </row>
     <row r="32" spans="1:18" ht="21">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3860,16 +3937,16 @@
       <c r="C32" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>279</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -3887,10 +3964,10 @@
       <c r="M32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O32" s="7"/>
+      <c r="O32" s="6"/>
     </row>
     <row r="33" spans="1:18" ht="21">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>190</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3899,16 +3976,16 @@
       <c r="C33" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="14" t="s">
         <v>404</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -3944,25 +4021,25 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="21">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="8" t="s">
         <v>227</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -3980,31 +4057,31 @@
       <c r="L34" s="2"/>
       <c r="M34" s="1"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="7"/>
+      <c r="O34" s="6"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="3"/>
     </row>
     <row r="35" spans="1:18" ht="21">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="4" t="s">
         <v>228</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -4022,31 +4099,31 @@
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="7"/>
+      <c r="O35" s="6"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="3"/>
     </row>
     <row r="36" spans="1:18" ht="21">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>191</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="7" t="s">
         <v>280</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -4080,7 +4157,7 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="21">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>191</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -4089,16 +4166,16 @@
       <c r="C37" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="7" t="s">
         <v>229</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -4118,13 +4195,13 @@
         <v>13</v>
       </c>
       <c r="N37" s="1"/>
-      <c r="O37" s="7"/>
+      <c r="O37" s="6"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="3"/>
     </row>
     <row r="38" spans="1:18" ht="21">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>191</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -4133,16 +4210,16 @@
       <c r="C38" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="7" t="s">
         <v>230</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -4162,31 +4239,31 @@
         <v>13</v>
       </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="7"/>
+      <c r="O38" s="6"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="3"/>
     </row>
     <row r="39" spans="1:18" ht="21">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="7" t="s">
         <v>231</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -4218,7 +4295,7 @@
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="1:18" ht="21">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>192</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -4227,7 +4304,7 @@
       <c r="C40" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -4244,13 +4321,13 @@
       <c r="L40" s="2"/>
       <c r="M40" s="1"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="7"/>
+      <c r="O40" s="6"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
     <row r="41" spans="1:18" ht="21">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>192</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -4259,7 +4336,7 @@
       <c r="C41" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -4276,31 +4353,31 @@
       <c r="L41" s="2"/>
       <c r="M41" s="1"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="7"/>
+      <c r="O41" s="6"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
     </row>
     <row r="42" spans="1:18" ht="21">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>406</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G42" s="14" t="s">
         <v>405</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -4338,7 +4415,7 @@
       </c>
     </row>
     <row r="43" spans="1:18" ht="21">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -4347,7 +4424,7 @@
       <c r="C43" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -4366,13 +4443,13 @@
       <c r="L43" s="2"/>
       <c r="M43" s="1"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="7"/>
+      <c r="O43" s="6"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="3"/>
     </row>
     <row r="44" spans="1:18" ht="21">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -4381,7 +4458,7 @@
       <c r="C44" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -4400,13 +4477,13 @@
       <c r="L44" s="2"/>
       <c r="M44" s="1"/>
       <c r="N44" s="2"/>
-      <c r="O44" s="7"/>
+      <c r="O44" s="6"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="3"/>
     </row>
     <row r="45" spans="1:18" ht="21">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -4415,7 +4492,7 @@
       <c r="C45" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -4434,13 +4511,13 @@
       <c r="L45" s="2"/>
       <c r="M45" s="1"/>
       <c r="N45" s="2"/>
-      <c r="O45" s="7"/>
+      <c r="O45" s="6"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="3"/>
     </row>
     <row r="46" spans="1:18" ht="21">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -4449,7 +4526,7 @@
       <c r="C46" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -4468,13 +4545,13 @@
       <c r="L46" s="2"/>
       <c r="M46" s="1"/>
       <c r="N46" s="2"/>
-      <c r="O46" s="7"/>
+      <c r="O46" s="6"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="3"/>
     </row>
     <row r="47" spans="1:18" ht="21">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -4483,13 +4560,13 @@
       <c r="C47" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G47" s="9"/>
+      <c r="G47" s="8"/>
       <c r="H47" s="1" t="s">
         <v>10</v>
       </c>
@@ -4503,13 +4580,13 @@
       <c r="L47" s="2"/>
       <c r="M47" s="1"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="7"/>
+      <c r="O47" s="6"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="3"/>
     </row>
     <row r="48" spans="1:18" ht="21">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -4518,13 +4595,13 @@
       <c r="C48" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G48" s="9"/>
+      <c r="G48" s="8"/>
       <c r="H48" s="1" t="s">
         <v>10</v>
       </c>
@@ -4538,13 +4615,13 @@
       <c r="L48" s="2"/>
       <c r="M48" s="1"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="7"/>
+      <c r="O48" s="6"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="3"/>
     </row>
     <row r="49" spans="1:18" ht="21">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -4553,16 +4630,16 @@
       <c r="C49" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="14" t="s">
         <v>416</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -4596,7 +4673,7 @@
       </c>
     </row>
     <row r="50" spans="1:18" ht="21">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4605,13 +4682,13 @@
       <c r="C50" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G50" s="9"/>
+      <c r="G50" s="8"/>
       <c r="H50" s="1" t="s">
         <v>10</v>
       </c>
@@ -4623,13 +4700,13 @@
       <c r="L50" s="2"/>
       <c r="M50" s="1"/>
       <c r="N50" s="2"/>
-      <c r="O50" s="7"/>
+      <c r="O50" s="6"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="3"/>
     </row>
     <row r="51" spans="1:18" ht="21">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -4638,13 +4715,13 @@
       <c r="C51" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G51" s="9"/>
+      <c r="G51" s="8"/>
       <c r="H51" s="1" t="s">
         <v>10</v>
       </c>
@@ -4656,13 +4733,13 @@
       <c r="L51" s="2"/>
       <c r="M51" s="1"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="7"/>
+      <c r="O51" s="6"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="3"/>
     </row>
     <row r="52" spans="1:18" ht="21">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -4671,13 +4748,13 @@
       <c r="C52" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G52" s="9"/>
+      <c r="G52" s="8"/>
       <c r="H52" s="1" t="s">
         <v>10</v>
       </c>
@@ -4689,13 +4766,13 @@
       <c r="L52" s="2"/>
       <c r="M52" s="1"/>
       <c r="N52" s="2"/>
-      <c r="O52" s="7"/>
+      <c r="O52" s="6"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="3"/>
     </row>
     <row r="53" spans="1:18" ht="21">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -4704,13 +4781,13 @@
       <c r="C53" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="9"/>
+      <c r="G53" s="8"/>
       <c r="H53" s="1" t="s">
         <v>10</v>
       </c>
@@ -4722,13 +4799,13 @@
       <c r="L53" s="2"/>
       <c r="M53" s="1"/>
       <c r="N53" s="2"/>
-      <c r="O53" s="7"/>
+      <c r="O53" s="6"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="3"/>
     </row>
     <row r="54" spans="1:18" ht="21">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -4737,13 +4814,13 @@
       <c r="C54" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D54" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G54" s="9"/>
+      <c r="G54" s="8"/>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
@@ -4755,31 +4832,31 @@
       <c r="L54" s="2"/>
       <c r="M54" s="1"/>
       <c r="N54" s="2"/>
-      <c r="O54" s="7"/>
+      <c r="O54" s="6"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="3"/>
     </row>
     <row r="55" spans="1:18" ht="21">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>195</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="16" t="s">
         <v>431</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E55" s="9" t="s">
+      <c r="D55" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G55" s="30" t="s">
+      <c r="G55" s="27" t="s">
         <v>457</v>
       </c>
       <c r="H55" s="2" t="s">
@@ -4788,7 +4865,7 @@
       <c r="I55" s="2">
         <v>25</v>
       </c>
-      <c r="J55" s="9" t="s">
+      <c r="J55" s="8" t="s">
         <v>207</v>
       </c>
       <c r="K55" s="2" t="s">
@@ -4813,276 +4890,280 @@
       </c>
     </row>
     <row r="56" spans="1:18" ht="21">
-      <c r="A56" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>432</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E56" s="9" t="s">
+      <c r="A56" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>460</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F56" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>381</v>
+      <c r="F56" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G56" s="30" t="s">
+        <v>466</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I56" s="2">
-        <v>15</v>
-      </c>
-      <c r="J56" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K56" s="2">
-        <v>15</v>
+      <c r="K56" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="L56" s="2"/>
       <c r="M56" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N56" s="2" t="s">
-        <v>263</v>
+      <c r="N56" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="P56" s="19" t="s">
-        <v>88</v>
+        <v>463</v>
+      </c>
+      <c r="P56" t="s">
+        <v>465</v>
       </c>
       <c r="Q56" s="2"/>
-      <c r="R56" s="2" t="s">
-        <v>55</v>
+      <c r="R56" s="29" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="21">
-      <c r="A57" s="7" t="s">
-        <v>197</v>
+      <c r="A57" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>383</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E57" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>384</v>
+      <c r="F57" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I57" s="2">
-        <v>14</v>
-      </c>
-      <c r="J57" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K57" s="2" t="s">
-        <v>174</v>
+      <c r="K57" s="2">
+        <v>15</v>
       </c>
       <c r="L57" s="2"/>
       <c r="M57" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>86</v>
+        <v>244</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
+      <c r="R57" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="58" spans="1:18" ht="21">
-      <c r="A58" s="7" t="s">
-        <v>198</v>
+      <c r="A58" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>433</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E58" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E58" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F58" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>232</v>
+      <c r="F58" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>384</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I58" s="2">
-        <v>12</v>
-      </c>
-      <c r="J58" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K58" s="2">
-        <v>12</v>
+      <c r="K58" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="L58" s="2"/>
       <c r="M58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="Q58" s="2"/>
-      <c r="R58" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="R58" s="2"/>
     </row>
     <row r="59" spans="1:18" ht="21">
-      <c r="A59" s="7" t="s">
-        <v>199</v>
+      <c r="A59" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E59" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F59" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>281</v>
+      <c r="F59" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I59" s="2">
-        <v>4</v>
-      </c>
-      <c r="J59" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>207</v>
+      </c>
       <c r="K59" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L59" s="2"/>
       <c r="M59" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
+      <c r="R59" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="60" spans="1:18" ht="21">
-      <c r="A60" s="7" t="s">
-        <v>200</v>
+      <c r="A60" s="6" t="s">
+        <v>199</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>414</v>
+        <v>60</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="I60" s="2">
-        <v>25</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>174</v>
+        <v>4</v>
+      </c>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2">
+        <v>4</v>
       </c>
       <c r="L60" s="2"/>
       <c r="M60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N60" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>266</v>
+      </c>
       <c r="O60" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="P60" s="2" t="s">
-        <v>87</v>
+        <v>245</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
     <row r="61" spans="1:18" ht="21">
-      <c r="A61" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>422</v>
-      </c>
-      <c r="D61" s="9" t="s">
+      <c r="A61" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F61" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="G61" s="15" t="s">
-        <v>415</v>
+      <c r="F61" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>414</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>10</v>
@@ -5111,1091 +5192,1178 @@
       <c r="R61" s="2"/>
     </row>
     <row r="62" spans="1:18" ht="21">
-      <c r="A62" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>233</v>
+      <c r="A62" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>415</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="I62" s="2">
-        <v>15</v>
-      </c>
-      <c r="J62" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="K62" s="2">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N62" s="2" t="s">
-        <v>267</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="N62" s="2"/>
       <c r="O62" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="P62" s="20" t="s">
-        <v>137</v>
+        <v>241</v>
+      </c>
+      <c r="P62" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q62" s="2"/>
-      <c r="R62" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="R62" s="2"/>
     </row>
     <row r="63" spans="1:18" ht="21">
-      <c r="A63" s="7" t="s">
-        <v>202</v>
+      <c r="A63" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E63" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E63" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F63" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G63" s="15" t="s">
-        <v>380</v>
+      <c r="F63" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>233</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I63" s="2">
-        <v>8</v>
-      </c>
-      <c r="J63" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="8" t="s">
         <v>207</v>
       </c>
       <c r="K63" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="P63" s="1" t="s">
-        <v>176</v>
+        <v>250</v>
+      </c>
+      <c r="P63" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
+      <c r="R63" s="2" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="64" spans="1:18" ht="21">
-      <c r="A64" s="7" t="s">
-        <v>203</v>
+      <c r="A64" s="6" t="s">
+        <v>202</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E64" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F64" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>234</v>
+      <c r="F64" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>380</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="I64" s="2">
-        <v>16</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>174</v>
+        <v>8</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K64" s="2">
+        <v>8</v>
       </c>
       <c r="L64" s="2"/>
       <c r="M64" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N64" s="2"/>
-      <c r="O64" s="7"/>
-      <c r="P64" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q64" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="R64" s="2" t="s">
-        <v>89</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="O64" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
     </row>
     <row r="65" spans="1:18" ht="21">
-      <c r="A65" s="7" t="s">
-        <v>204</v>
+      <c r="A65" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>425</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E65" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F65" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="G65" s="10" t="s">
-        <v>305</v>
+      <c r="F65" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="I65" s="2">
-        <v>15</v>
-      </c>
-      <c r="J65" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="K65" s="2">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="L65" s="2"/>
       <c r="M65" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="O65" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="P65" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q65" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q65" s="17" t="s">
+        <v>139</v>
+      </c>
       <c r="R65" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="21">
-      <c r="A66" s="7" t="s">
-        <v>205</v>
+      <c r="A66" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E66" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F66" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G66" s="15" t="s">
-        <v>235</v>
+      <c r="F66" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>305</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I66" s="2">
+        <v>15</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K66" s="2">
+        <v>15</v>
+      </c>
+      <c r="L66" s="2"/>
+      <c r="M66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="O66" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="P66" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="21">
+      <c r="A67" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="2">
         <v>12</v>
       </c>
-      <c r="J66" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K66" s="2" t="s">
+      <c r="J67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K67" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2" t="s">
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="O66" s="3" t="s">
+      <c r="O67" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="2"/>
-    </row>
-    <row r="67" spans="1:18" ht="21">
-      <c r="A67" s="7" t="s">
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="2"/>
+    </row>
+    <row r="68" spans="1:18" ht="21">
+      <c r="A68" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B68" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C68" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="D67" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E67" s="11" t="s">
+      <c r="D68" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F68" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G68" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="H67" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J67" s="9" t="s">
+      <c r="H68" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J68" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K67" s="5" t="s">
+      <c r="K68" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="M67" s="1" t="s">
+      <c r="M68" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="N67" s="3" t="s">
+      <c r="N68" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="O67" s="3" t="s">
+      <c r="O68" s="3" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="21">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:18" ht="21">
+      <c r="A69" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B69" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C69" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="D68" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E68" s="12" t="s">
+      <c r="D69" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F69" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="G69" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="H68" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N68" s="3" t="s">
+      <c r="H69" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N69" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="O68" s="3" t="s">
+      <c r="O69" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="21">
-      <c r="A69" s="7" t="s">
+    <row r="70" spans="1:18" ht="21">
+      <c r="A70" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B70" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C70" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="D69" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E69" s="12" t="s">
+      <c r="D70" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F70" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="G69" s="15" t="s">
+      <c r="G70" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="H69" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N69" s="3" t="s">
+      <c r="H70" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N70" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="O69" s="3" t="s">
+      <c r="O70" s="3" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="21">
-      <c r="A70" s="7" t="s">
+    <row r="71" spans="1:18" ht="21">
+      <c r="A71" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B71" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C71" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D71" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E71" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F71" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="G70" s="12" t="s">
+      <c r="G71" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="H70" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N70" s="3" t="s">
+      <c r="H71" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N71" s="3" t="s">
         <v>368</v>
-      </c>
-      <c r="O70" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" ht="21">
-      <c r="A71" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="H71" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N71" s="3" t="s">
-        <v>367</v>
       </c>
       <c r="O71" s="3" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="21">
-      <c r="A72" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>435</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="G72" s="15" t="s">
-        <v>418</v>
-      </c>
-      <c r="H72" s="12" t="s">
+      <c r="A72" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="H72" s="11" t="s">
         <v>10</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="O72" s="3" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="21">
-      <c r="A73" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="E73" s="12" t="s">
+      <c r="A73" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F73" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="H73" s="12" t="s">
+      <c r="F73" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="H73" s="11" t="s">
         <v>10</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="O73" s="3" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="21">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="O74" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="21">
+      <c r="A75" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B75" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="D74" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E74" s="12" t="s">
+      <c r="D75" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F74" s="14" t="s">
+      <c r="F75" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G75" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="H74" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N74" s="3" t="s">
+      <c r="H75" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N75" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="O74" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="P74" s="21" t="s">
-        <v>437</v>
-      </c>
-      <c r="Q74" s="5" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" ht="21">
-      <c r="A75" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F75" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="G75" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="H75" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N75" s="3" t="s">
-        <v>363</v>
       </c>
       <c r="O75" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="P75" s="21" t="s">
-        <v>438</v>
-      </c>
-      <c r="Q75" s="5" t="s">
-        <v>436</v>
+      <c r="P75" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q75" s="4" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="21">
-      <c r="A76" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E76" s="12" t="s">
+      <c r="A76" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E76" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F76" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="H76" s="12" t="s">
+      <c r="F76" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="H76" s="11" t="s">
         <v>10</v>
       </c>
       <c r="N76" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="O76" s="3" t="s">
         <v>372</v>
       </c>
+      <c r="P76" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q76" s="4" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="77" spans="1:18" ht="21">
-      <c r="A77" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E77" s="12" t="s">
+      <c r="A77" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F77" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="H77" s="12" t="s">
+      <c r="F77" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="H77" s="11" t="s">
         <v>10</v>
       </c>
       <c r="N77" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="O77" s="3" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="21">
-      <c r="A78" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E78" s="12" t="s">
+      <c r="A78" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E78" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F78" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="H78" s="12" t="s">
+      <c r="F78" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="H78" s="11" t="s">
         <v>10</v>
       </c>
       <c r="N78" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="O78" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="P78" s="22" t="s">
+    </row>
+    <row r="79" spans="1:18" ht="21">
+      <c r="A79" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="H79" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N79" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="O79" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="P79" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="Q78" s="5" t="s">
+      <c r="Q79" s="4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="26" customFormat="1" ht="63">
-      <c r="A79" s="24" t="s">
+    <row r="80" spans="1:18" s="23" customFormat="1" ht="63">
+      <c r="A80" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="B79" s="25" t="s">
+      <c r="B80" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="C79" s="25" t="s">
+      <c r="C80" s="22" t="s">
         <v>446</v>
       </c>
-      <c r="D79" s="26" t="s">
+      <c r="D80" s="23" t="s">
         <v>447</v>
       </c>
-      <c r="E79" s="27" t="s">
+      <c r="E80" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F79" s="26" t="s">
+      <c r="F80" s="23" t="s">
         <v>448</v>
       </c>
-      <c r="G79" s="26" t="s">
+      <c r="G80" s="23" t="s">
         <v>449</v>
       </c>
-      <c r="H79" s="27"/>
-      <c r="M79" s="1" t="s">
+      <c r="H80" s="24"/>
+      <c r="M80" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N79" s="28" t="s">
+      <c r="N80" s="25" t="s">
         <v>443</v>
       </c>
-      <c r="O79" s="28" t="s">
+      <c r="O80" s="25" t="s">
         <v>372</v>
       </c>
-      <c r="P79" s="29" t="s">
+      <c r="P80" s="26" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="23.25">
-      <c r="A80" s="13" t="s">
+    <row r="81" spans="1:18" ht="23.25">
+      <c r="A81" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C81" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E80" s="12" t="s">
+      <c r="D81" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F81" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="G81" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="H80" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N80" s="3" t="s">
+      <c r="H81" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N81" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="O80" s="3" t="s">
+      <c r="O81" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="P80" s="23" t="s">
+      <c r="P81" s="20" t="s">
         <v>440</v>
       </c>
-      <c r="R80" s="5" t="s">
+      <c r="R81" s="4" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="23.25">
-      <c r="A81" s="13" t="s">
+    <row r="82" spans="1:18" ht="23.25">
+      <c r="A82" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H81" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" ht="23.25">
-      <c r="A82" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D82" s="9" t="s">
+      <c r="D82" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H82" s="12" t="s">
+      <c r="H82" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="23.25">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="12" t="s">
         <v>342</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D83" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H83" s="12" t="s">
+      <c r="H83" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="23.25">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="12" t="s">
         <v>342</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D84" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H84" s="12" t="s">
+      <c r="H84" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="23.25">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="12" t="s">
         <v>342</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D85" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>210</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H85" s="12" t="s">
+      <c r="H85" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="23.25">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H86" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="23.25">
+      <c r="A87" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B87" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C87" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E86" s="12" t="s">
+      <c r="D87" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E87" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F87" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="G86" s="5" t="s">
+      <c r="G87" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="H86" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N86" s="3" t="s">
+      <c r="H87" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N87" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="O86" s="3" t="s">
+      <c r="O87" s="3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="21">
-      <c r="A87" s="7" t="s">
+    <row r="88" spans="1:18" ht="21">
+      <c r="A88" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B88" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C88" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="D87" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E87" s="12" t="s">
+      <c r="D88" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E88" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F88" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="G87" s="15" t="s">
+      <c r="G88" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="H87" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N87" s="3" t="s">
+      <c r="H88" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N88" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="O87" s="3" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" ht="21">
-      <c r="A88" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" s="16" t="s">
-        <v>390</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="H88" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N88" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="O88" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="P88" s="16" t="s">
+    </row>
+    <row r="89" spans="1:18" ht="21">
+      <c r="A89" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="O89" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="P89" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="Q88" s="5" t="s">
+      <c r="Q89" s="4" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="21">
-      <c r="A89" s="7" t="s">
+    <row r="90" spans="1:18" ht="21">
+      <c r="A90" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B89" s="30" t="s">
+      <c r="B90" s="27" t="s">
         <v>451</v>
       </c>
-      <c r="C89" s="30" t="s">
+      <c r="C90" s="27" t="s">
         <v>452</v>
       </c>
-      <c r="D89" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E89" s="9" t="s">
+      <c r="D90" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E90" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="F90" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="G89" s="30" t="s">
+      <c r="G90" s="27" t="s">
         <v>456</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I89" s="2">
+      <c r="I90" s="2">
         <v>25</v>
       </c>
-      <c r="J89" s="9" t="s">
+      <c r="J90" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="K90" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="L89" s="2"/>
-      <c r="M89" s="1" t="s">
+      <c r="L90" s="2"/>
+      <c r="M90" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N89" s="3" t="s">
+      <c r="N90" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="O89" s="3" t="s">
+      <c r="O90" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="P89" s="1"/>
-      <c r="Q89" s="2"/>
-      <c r="R89" s="1"/>
-    </row>
-    <row r="95" spans="1:18">
-      <c r="G95" s="9"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="2"/>
+      <c r="R90" s="1"/>
+    </row>
+    <row r="91" spans="1:18" s="23" customFormat="1" ht="128.25">
+      <c r="A91" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="E91" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="G91" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="H91" s="24"/>
+      <c r="M91" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="N91" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="O91" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="P91" s="31" t="s">
+        <v>474</v>
+      </c>
+      <c r="R91" s="23" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="96" spans="1:18">
-      <c r="G96" s="9"/>
-    </row>
-    <row r="103" spans="7:7">
-      <c r="G103" s="9"/>
+      <c r="G96" s="8"/>
+    </row>
+    <row r="97" spans="7:7">
+      <c r="G97" s="8"/>
     </row>
     <row r="104" spans="7:7">
-      <c r="G104" s="9"/>
+      <c r="G104" s="8"/>
     </row>
     <row r="105" spans="7:7">
-      <c r="G105" s="9"/>
-    </row>
-    <row r="110" spans="7:7">
-      <c r="G110" s="9"/>
+      <c r="G105" s="8"/>
+    </row>
+    <row r="106" spans="7:7">
+      <c r="G106" s="8"/>
     </row>
     <row r="111" spans="7:7">
-      <c r="G111" s="9"/>
+      <c r="G111" s="8"/>
     </row>
     <row r="112" spans="7:7">
-      <c r="G112" s="9"/>
+      <c r="G112" s="8"/>
     </row>
     <row r="113" spans="7:7">
-      <c r="G113" s="9"/>
+      <c r="G113" s="8"/>
     </row>
     <row r="114" spans="7:7">
-      <c r="G114" s="9"/>
+      <c r="G114" s="8"/>
     </row>
     <row r="115" spans="7:7">
-      <c r="G115" s="9"/>
+      <c r="G115" s="8"/>
     </row>
     <row r="116" spans="7:7">
-      <c r="G116" s="9"/>
+      <c r="G116" s="8"/>
     </row>
     <row r="117" spans="7:7">
-      <c r="G117" s="9"/>
+      <c r="G117" s="8"/>
     </row>
     <row r="118" spans="7:7">
-      <c r="G118" s="9"/>
-    </row>
-    <row r="122" spans="7:7">
-      <c r="G122" s="9"/>
+      <c r="G118" s="8"/>
+    </row>
+    <row r="119" spans="7:7">
+      <c r="G119" s="8"/>
     </row>
     <row r="123" spans="7:7">
-      <c r="G123" s="9"/>
+      <c r="G123" s="8"/>
     </row>
     <row r="124" spans="7:7">
-      <c r="G124" s="9"/>
+      <c r="G124" s="8"/>
     </row>
     <row r="125" spans="7:7">
-      <c r="G125" s="9"/>
+      <c r="G125" s="8"/>
     </row>
     <row r="126" spans="7:7">
-      <c r="G126" s="9"/>
+      <c r="G126" s="8"/>
     </row>
     <row r="127" spans="7:7">
-      <c r="G127" s="9"/>
+      <c r="G127" s="8"/>
     </row>
     <row r="128" spans="7:7">
-      <c r="G128" s="9"/>
+      <c r="G128" s="8"/>
     </row>
     <row r="129" spans="7:7">
-      <c r="G129" s="9"/>
+      <c r="G129" s="8"/>
     </row>
     <row r="130" spans="7:7">
-      <c r="G130" s="9"/>
+      <c r="G130" s="8"/>
     </row>
     <row r="131" spans="7:7">
-      <c r="G131" s="9"/>
+      <c r="G131" s="8"/>
     </row>
     <row r="132" spans="7:7">
-      <c r="G132" s="9"/>
+      <c r="G132" s="8"/>
     </row>
     <row r="133" spans="7:7">
-      <c r="G133" s="9"/>
+      <c r="G133" s="8"/>
     </row>
     <row r="134" spans="7:7">
-      <c r="G134" s="9"/>
+      <c r="G134" s="8"/>
     </row>
     <row r="135" spans="7:7">
-      <c r="G135" s="9"/>
+      <c r="G135" s="8"/>
     </row>
     <row r="136" spans="7:7">
-      <c r="G136" s="9"/>
+      <c r="G136" s="8"/>
     </row>
     <row r="137" spans="7:7">
-      <c r="G137" s="9"/>
+      <c r="G137" s="8"/>
     </row>
     <row r="138" spans="7:7">
-      <c r="G138" s="9"/>
+      <c r="G138" s="8"/>
     </row>
     <row r="139" spans="7:7">
-      <c r="G139" s="9"/>
+      <c r="G139" s="8"/>
     </row>
     <row r="140" spans="7:7">
-      <c r="G140" s="9"/>
+      <c r="G140" s="8"/>
+    </row>
+    <row r="141" spans="7:7">
+      <c r="G141" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="R17" r:id="rId1" xr:uid="{C72C4340-8EFA-9F4E-BD08-539B76505C50}"/>
     <hyperlink ref="R23" r:id="rId2" xr:uid="{BCB215EC-5FC7-584B-8854-B6AEC003D70A}"/>
@@ -6218,56 +6386,60 @@
     <hyperlink ref="O39" r:id="rId19" xr:uid="{44CAB423-567B-4F9A-B424-F4A45325DDB2}"/>
     <hyperlink ref="O42" r:id="rId20" xr:uid="{2F441EEB-5162-4DC9-A095-E6A33F4B96A7}"/>
     <hyperlink ref="O49" r:id="rId21" xr:uid="{EC443C3A-7836-4460-83D0-5C73F759181A}"/>
-    <hyperlink ref="O55" r:id="rId22" xr:uid="{AA15EF38-43FE-4806-AD37-C00D4F12DA14}"/>
-    <hyperlink ref="O58" r:id="rId23" xr:uid="{70FB95CD-A9C5-4BE0-AEE3-E3338FA20098}"/>
-    <hyperlink ref="O62" r:id="rId24" xr:uid="{177009B3-D672-4BC0-8A69-947FBF783793}"/>
-    <hyperlink ref="O65" r:id="rId25" xr:uid="{117C7FE1-97AB-4954-AE8D-1AD48BD864F8}"/>
-    <hyperlink ref="O56" r:id="rId26" xr:uid="{FBEBC241-67BD-40C0-8CA9-ABBB5A964CDF}"/>
-    <hyperlink ref="O57" r:id="rId27" xr:uid="{E3AFAD2B-9AE4-4D18-8B98-449BA7D471F3}"/>
-    <hyperlink ref="O59" r:id="rId28" xr:uid="{4AB2DAB5-6B75-435A-9541-C298B0E18588}"/>
-    <hyperlink ref="O63" r:id="rId29" xr:uid="{FE3E304A-8501-47E8-BCC9-30FD14B226DF}"/>
-    <hyperlink ref="O66" r:id="rId30" xr:uid="{D6486464-2243-4229-B25B-05676D833C2D}"/>
-    <hyperlink ref="O60" r:id="rId31" xr:uid="{601B5599-7C00-4021-ABB4-2A5CB3D4982A}"/>
-    <hyperlink ref="O61" r:id="rId32" xr:uid="{82C7F15A-0905-474E-B047-A7BB4379FCA8}"/>
-    <hyperlink ref="N67" r:id="rId33" xr:uid="{BF935FA2-E37D-4CA8-8536-DD8CA66BE7FD}"/>
-    <hyperlink ref="O67" r:id="rId34" xr:uid="{B6A64B24-F697-4591-8B4B-26653811AD6E}"/>
-    <hyperlink ref="N68" r:id="rId35" xr:uid="{7AA65321-1918-4211-99D0-DDDD2957D86A}"/>
-    <hyperlink ref="N69" r:id="rId36" xr:uid="{1CF38881-58BD-4F74-9AF9-0748346A41AB}"/>
-    <hyperlink ref="N70" r:id="rId37" xr:uid="{73252989-590E-46C6-A34D-FFBEE619DE18}"/>
-    <hyperlink ref="N71" r:id="rId38" xr:uid="{7785D349-BF49-4491-8D31-044A9762A2E5}"/>
-    <hyperlink ref="N72" r:id="rId39" xr:uid="{7C1629DE-0279-4F05-BBF3-048BAF41A4BC}"/>
-    <hyperlink ref="N73" r:id="rId40" xr:uid="{F1CD9645-60C6-4569-9CB5-EEDE71AE2A83}"/>
-    <hyperlink ref="N74" r:id="rId41" xr:uid="{85CFDEAB-3345-4554-9E19-D2435FE6B424}"/>
-    <hyperlink ref="N75" r:id="rId42" xr:uid="{9A265FA2-F389-4520-A5F4-DA4BAE1B5417}"/>
-    <hyperlink ref="N76" r:id="rId43" xr:uid="{085DF4E6-0857-4F52-B888-AB2AA65C8E11}"/>
-    <hyperlink ref="N77" r:id="rId44" xr:uid="{C2D445B9-1683-436A-AA87-7CE4E2D2B129}"/>
-    <hyperlink ref="N78" r:id="rId45" xr:uid="{5D55D737-5EEE-4A44-9266-74EFB0F6A55B}"/>
-    <hyperlink ref="N80" r:id="rId46" xr:uid="{719C0F73-D177-4FC7-A032-E81D845F0146}"/>
-    <hyperlink ref="N86" r:id="rId47" xr:uid="{2D5B57D7-4E19-402F-A3D1-0190D1D111E9}"/>
-    <hyperlink ref="N87" r:id="rId48" xr:uid="{2A8A5E7D-6F75-435C-8798-DADA79207756}"/>
-    <hyperlink ref="N88" r:id="rId49" xr:uid="{046E1E83-08DD-4ABD-BE67-51826BD94B40}"/>
-    <hyperlink ref="O68" r:id="rId50" xr:uid="{14DAF574-A575-4913-97D6-38E4F9A36D4C}"/>
-    <hyperlink ref="O69" r:id="rId51" xr:uid="{26C01D2D-D88D-4CED-8216-CFA5AB9F6B5C}"/>
-    <hyperlink ref="O70" r:id="rId52" xr:uid="{F233D98D-6C14-4E46-8903-114F3B2E7739}"/>
-    <hyperlink ref="O71" r:id="rId53" xr:uid="{EC310FAA-84BF-4E0E-92E5-EE244577AF79}"/>
-    <hyperlink ref="O72" r:id="rId54" xr:uid="{1E2C866D-C13F-4B54-A20B-D5E421419C19}"/>
-    <hyperlink ref="O73" r:id="rId55" xr:uid="{447A9882-6201-4486-83F3-EF15DC5A23B5}"/>
-    <hyperlink ref="O80" r:id="rId56" xr:uid="{257548C8-8554-4760-850B-FC1770457B9B}"/>
-    <hyperlink ref="O86" r:id="rId57" xr:uid="{9400E53B-43FA-4DE0-A03E-E5942B254DA7}"/>
-    <hyperlink ref="O74" r:id="rId58" xr:uid="{D0C3DB44-1D89-43D7-925A-2A8213C2FC99}"/>
-    <hyperlink ref="O75" r:id="rId59" xr:uid="{9060BDD3-10ED-486F-919B-7C46AB43CE72}"/>
-    <hyperlink ref="O76" r:id="rId60" xr:uid="{57D64F97-E371-41B8-8C86-1DD27711CEED}"/>
-    <hyperlink ref="O77" r:id="rId61" xr:uid="{BE31E0FB-6FDD-4A16-B1A6-D967EBBA604D}"/>
-    <hyperlink ref="O78" r:id="rId62" xr:uid="{932F5256-5AF7-47C3-93E7-D4FFD6CEE619}"/>
-    <hyperlink ref="O87" r:id="rId63" xr:uid="{4B94D87A-2556-4E8B-BFF8-B4465BDF0633}"/>
-    <hyperlink ref="O88" r:id="rId64" xr:uid="{82BCE4C9-D795-4AB2-9202-309AD9F062A0}"/>
+    <hyperlink ref="O56" r:id="rId22" xr:uid="{AA15EF38-43FE-4806-AD37-C00D4F12DA14}"/>
+    <hyperlink ref="O59" r:id="rId23" xr:uid="{70FB95CD-A9C5-4BE0-AEE3-E3338FA20098}"/>
+    <hyperlink ref="O63" r:id="rId24" xr:uid="{177009B3-D672-4BC0-8A69-947FBF783793}"/>
+    <hyperlink ref="O66" r:id="rId25" xr:uid="{117C7FE1-97AB-4954-AE8D-1AD48BD864F8}"/>
+    <hyperlink ref="O57" r:id="rId26" xr:uid="{FBEBC241-67BD-40C0-8CA9-ABBB5A964CDF}"/>
+    <hyperlink ref="O58" r:id="rId27" xr:uid="{E3AFAD2B-9AE4-4D18-8B98-449BA7D471F3}"/>
+    <hyperlink ref="O60" r:id="rId28" xr:uid="{4AB2DAB5-6B75-435A-9541-C298B0E18588}"/>
+    <hyperlink ref="O64" r:id="rId29" xr:uid="{FE3E304A-8501-47E8-BCC9-30FD14B226DF}"/>
+    <hyperlink ref="O67" r:id="rId30" xr:uid="{D6486464-2243-4229-B25B-05676D833C2D}"/>
+    <hyperlink ref="O61" r:id="rId31" xr:uid="{601B5599-7C00-4021-ABB4-2A5CB3D4982A}"/>
+    <hyperlink ref="O62" r:id="rId32" xr:uid="{82C7F15A-0905-474E-B047-A7BB4379FCA8}"/>
+    <hyperlink ref="N68" r:id="rId33" xr:uid="{BF935FA2-E37D-4CA8-8536-DD8CA66BE7FD}"/>
+    <hyperlink ref="O68" r:id="rId34" xr:uid="{B6A64B24-F697-4591-8B4B-26653811AD6E}"/>
+    <hyperlink ref="N69" r:id="rId35" xr:uid="{7AA65321-1918-4211-99D0-DDDD2957D86A}"/>
+    <hyperlink ref="N70" r:id="rId36" xr:uid="{1CF38881-58BD-4F74-9AF9-0748346A41AB}"/>
+    <hyperlink ref="N71" r:id="rId37" xr:uid="{73252989-590E-46C6-A34D-FFBEE619DE18}"/>
+    <hyperlink ref="N72" r:id="rId38" xr:uid="{7785D349-BF49-4491-8D31-044A9762A2E5}"/>
+    <hyperlink ref="N73" r:id="rId39" xr:uid="{7C1629DE-0279-4F05-BBF3-048BAF41A4BC}"/>
+    <hyperlink ref="N74" r:id="rId40" xr:uid="{F1CD9645-60C6-4569-9CB5-EEDE71AE2A83}"/>
+    <hyperlink ref="N75" r:id="rId41" xr:uid="{85CFDEAB-3345-4554-9E19-D2435FE6B424}"/>
+    <hyperlink ref="N76" r:id="rId42" xr:uid="{9A265FA2-F389-4520-A5F4-DA4BAE1B5417}"/>
+    <hyperlink ref="N77" r:id="rId43" xr:uid="{085DF4E6-0857-4F52-B888-AB2AA65C8E11}"/>
+    <hyperlink ref="N78" r:id="rId44" xr:uid="{C2D445B9-1683-436A-AA87-7CE4E2D2B129}"/>
+    <hyperlink ref="N79" r:id="rId45" xr:uid="{5D55D737-5EEE-4A44-9266-74EFB0F6A55B}"/>
+    <hyperlink ref="N81" r:id="rId46" xr:uid="{719C0F73-D177-4FC7-A032-E81D845F0146}"/>
+    <hyperlink ref="N87" r:id="rId47" xr:uid="{2D5B57D7-4E19-402F-A3D1-0190D1D111E9}"/>
+    <hyperlink ref="N88" r:id="rId48" xr:uid="{2A8A5E7D-6F75-435C-8798-DADA79207756}"/>
+    <hyperlink ref="N89" r:id="rId49" xr:uid="{046E1E83-08DD-4ABD-BE67-51826BD94B40}"/>
+    <hyperlink ref="O69" r:id="rId50" xr:uid="{14DAF574-A575-4913-97D6-38E4F9A36D4C}"/>
+    <hyperlink ref="O70" r:id="rId51" xr:uid="{26C01D2D-D88D-4CED-8216-CFA5AB9F6B5C}"/>
+    <hyperlink ref="O71" r:id="rId52" xr:uid="{F233D98D-6C14-4E46-8903-114F3B2E7739}"/>
+    <hyperlink ref="O72" r:id="rId53" xr:uid="{EC310FAA-84BF-4E0E-92E5-EE244577AF79}"/>
+    <hyperlink ref="O73" r:id="rId54" xr:uid="{1E2C866D-C13F-4B54-A20B-D5E421419C19}"/>
+    <hyperlink ref="O74" r:id="rId55" xr:uid="{447A9882-6201-4486-83F3-EF15DC5A23B5}"/>
+    <hyperlink ref="O81" r:id="rId56" xr:uid="{257548C8-8554-4760-850B-FC1770457B9B}"/>
+    <hyperlink ref="O87" r:id="rId57" xr:uid="{9400E53B-43FA-4DE0-A03E-E5942B254DA7}"/>
+    <hyperlink ref="O75" r:id="rId58" xr:uid="{D0C3DB44-1D89-43D7-925A-2A8213C2FC99}"/>
+    <hyperlink ref="O76" r:id="rId59" xr:uid="{9060BDD3-10ED-486F-919B-7C46AB43CE72}"/>
+    <hyperlink ref="O77" r:id="rId60" xr:uid="{57D64F97-E371-41B8-8C86-1DD27711CEED}"/>
+    <hyperlink ref="O78" r:id="rId61" xr:uid="{BE31E0FB-6FDD-4A16-B1A6-D967EBBA604D}"/>
+    <hyperlink ref="O79" r:id="rId62" xr:uid="{932F5256-5AF7-47C3-93E7-D4FFD6CEE619}"/>
+    <hyperlink ref="O88" r:id="rId63" xr:uid="{4B94D87A-2556-4E8B-BFF8-B4465BDF0633}"/>
+    <hyperlink ref="O89" r:id="rId64" xr:uid="{82BCE4C9-D795-4AB2-9202-309AD9F062A0}"/>
     <hyperlink ref="R14" r:id="rId65" xr:uid="{83B92E27-A4C1-44FF-9FB3-FFFB798C2014}"/>
-    <hyperlink ref="N79" r:id="rId66" xr:uid="{18247FD7-8A34-4BF4-87E7-25ADE7E59731}"/>
+    <hyperlink ref="N80" r:id="rId66" xr:uid="{18247FD7-8A34-4BF4-87E7-25ADE7E59731}"/>
     <hyperlink ref="N39" r:id="rId67" xr:uid="{A113D5AA-DAD2-4191-B317-FAF70C3C58C0}"/>
-    <hyperlink ref="O89" r:id="rId68" xr:uid="{7F630C54-F0C0-4538-9138-0B92066BAC21}"/>
-    <hyperlink ref="N89" r:id="rId69" xr:uid="{6A004FC8-88CE-4E6C-9D03-7A09C5D6964F}"/>
+    <hyperlink ref="O90" r:id="rId68" xr:uid="{7F630C54-F0C0-4538-9138-0B92066BAC21}"/>
+    <hyperlink ref="N90" r:id="rId69" xr:uid="{6A004FC8-88CE-4E6C-9D03-7A09C5D6964F}"/>
+    <hyperlink ref="O55" r:id="rId70" xr:uid="{9B5A2A2F-2254-4CAE-9CBF-DA3418C2A3F0}"/>
+    <hyperlink ref="N56" r:id="rId71" xr:uid="{C30C6E6E-DEC6-4718-8BC0-AE5994F0E38D}"/>
+    <hyperlink ref="R56" r:id="rId72" xr:uid="{A61E19DF-7EFD-4303-9CA2-36D60E0608D2}"/>
+    <hyperlink ref="N91" r:id="rId73" xr:uid="{70712F6E-4E52-4699-953D-CADBD150BA3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId70"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added two test refs
</commit_message>
<xml_diff>
--- a/data/dots_test_def.xlsx
+++ b/data/dots_test_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rk/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\dots_home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F824D5-E9BD-7241-8A5F-F68D76421352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CEF8FA-3629-48BB-BA0E-B27BACF09D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="31580" windowHeight="19080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="506">
   <si>
     <t>name</t>
   </si>
@@ -2079,6 +2079,12 @@
   </si>
   <si>
     <t>https://link.springer.com/article/10.3758/s13428-022-01859-8</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.3758/s13428-023-02279-y</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/10.1177/20592043241257654</t>
   </si>
 </sst>
 </file>
@@ -2433,9 +2439,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2473,7 +2479,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2579,7 +2585,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2721,7 +2727,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2731,25 +2737,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P90" sqref="P90"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R70" sqref="R70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" style="1" customWidth="1"/>
     <col min="2" max="3" width="31.5" style="1" customWidth="1"/>
-    <col min="4" max="5" width="13.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
     <col min="9" max="10" width="20.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.625" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="23.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.125" style="1" customWidth="1"/>
     <col min="14" max="14" width="22.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="31.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="31.375" style="1" customWidth="1"/>
     <col min="16" max="16" width="19.5" style="1" customWidth="1"/>
     <col min="17" max="18" width="18.5" style="1" customWidth="1"/>
     <col min="19" max="1024" width="11" style="1"/>
@@ -5850,6 +5856,9 @@
       <c r="P70" s="27" t="s">
         <v>497</v>
       </c>
+      <c r="R70" s="22" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="71" spans="1:18" ht="21">
       <c r="A71" s="3" t="s">
@@ -6157,7 +6166,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="80" spans="1:18" s="13" customFormat="1" ht="68">
+    <row r="80" spans="1:18" s="13" customFormat="1" ht="63">
       <c r="A80" s="11" t="s">
         <v>422</v>
       </c>
@@ -6194,7 +6203,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="24">
+    <row r="81" spans="1:18" ht="23.25">
       <c r="A81" s="17" t="s">
         <v>430</v>
       </c>
@@ -6232,7 +6241,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="24">
+    <row r="82" spans="1:18" ht="23.25">
       <c r="A82" s="17" t="s">
         <v>430</v>
       </c>
@@ -6252,7 +6261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="24">
+    <row r="83" spans="1:18" ht="23.25">
       <c r="A83" s="17" t="s">
         <v>430</v>
       </c>
@@ -6272,7 +6281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="24">
+    <row r="84" spans="1:18" ht="23.25">
       <c r="A84" s="17" t="s">
         <v>430</v>
       </c>
@@ -6292,7 +6301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="24">
+    <row r="85" spans="1:18" ht="23.25">
       <c r="A85" s="17" t="s">
         <v>430</v>
       </c>
@@ -6312,7 +6321,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="24">
+    <row r="86" spans="1:18" ht="23.25">
       <c r="A86" s="17" t="s">
         <v>430</v>
       </c>
@@ -6332,7 +6341,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="24">
+    <row r="87" spans="1:18" ht="23.25">
       <c r="A87" s="17" t="s">
         <v>438</v>
       </c>
@@ -6483,9 +6492,11 @@
         <v>499</v>
       </c>
       <c r="Q90" s="4"/>
-      <c r="R90" s="4"/>
-    </row>
-    <row r="91" spans="1:18" s="13" customFormat="1" ht="135">
+      <c r="R90" s="22" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="13" customFormat="1" ht="128.25">
       <c r="A91" s="11" t="s">
         <v>464</v>
       </c>
@@ -6744,6 +6755,8 @@
     <hyperlink ref="N92" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
     <hyperlink ref="O92" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
     <hyperlink ref="R67" r:id="rId78" xr:uid="{FFB76916-3071-074B-99E1-093CC194DFE2}"/>
+    <hyperlink ref="R90" r:id="rId79" xr:uid="{F03C0612-F214-49AA-88B4-EFB9A3110C88}"/>
+    <hyperlink ref="R70" r:id="rId80" xr:uid="{BF99CB95-8732-461D-BBA6-6F0D17CAFA88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>